<commit_message>
Added scenario with maintenance costs, changed model for teh establsihment --> I need this version for the global model and the previous version for the the meta-analysis
</commit_message>
<xml_diff>
--- a/Data/mpatlas_export_nogeo_202503/Field_Definitions 2024_March2024.xlsx
+++ b/Data/mpatlas_export_nogeo_202503/Field_Definitions 2024_March2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bethp\Box Sync\GIS\Data Library\General\MPA Inventory\MPAtlas Exports\Current Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessiacosta/Desktop/PhD project/1. Thesis/Ch3. Costs of MPAs/Ch3-MPAcosts/Data/mpatlas_export_nogeo_202503/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD5ECD1-8AC5-4F21-8E47-4000BA97D475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B66049-3521-2E47-9513-55659C471857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MPAtlas Fields" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="296">
   <si>
     <t>protection_mpaguide_level</t>
   </si>
@@ -1186,6 +1186,9 @@
   </si>
   <si>
     <t xml:space="preserve">Based on the Regulation-Based Classification System. Learn more at https://www.classifympas.org/en/ </t>
+  </si>
+  <si>
+    <t>the assessment may have been modified by the author or another member of the MPAtlas team while updating or verifying the data.</t>
   </si>
 </sst>
 </file>
@@ -2191,29 +2194,29 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="37.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.83203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="61.83203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="71.83203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="34.59765625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.796875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="61.796875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="71.796875" style="5" customWidth="1"/>
     <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>196</v>
       </c>
@@ -2233,7 +2236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>187</v>
       </c>
@@ -2250,7 +2253,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>188</v>
       </c>
@@ -2267,7 +2270,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>189</v>
       </c>
@@ -2285,7 +2288,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>5</v>
       </c>
@@ -2303,7 +2306,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>8</v>
       </c>
@@ -2321,7 +2324,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>190</v>
       </c>
@@ -2339,7 +2342,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>191</v>
       </c>
@@ -2357,7 +2360,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>192</v>
       </c>
@@ -2375,7 +2378,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>12</v>
       </c>
@@ -2395,7 +2398,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>21</v>
       </c>
@@ -2415,7 +2418,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>136</v>
       </c>
@@ -2432,7 +2435,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>137</v>
       </c>
@@ -2449,7 +2452,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="69" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>16</v>
       </c>
@@ -2469,7 +2472,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>167</v>
       </c>
@@ -2486,7 +2489,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>168</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>138</v>
       </c>
@@ -2523,7 +2526,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
         <v>139</v>
       </c>
@@ -2540,7 +2543,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="51.75" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>140</v>
       </c>
@@ -2560,7 +2563,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
         <v>141</v>
       </c>
@@ -2578,7 +2581,7 @@
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="86.25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>135</v>
       </c>
@@ -2596,7 +2599,7 @@
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
         <v>150</v>
       </c>
@@ -2613,7 +2616,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
         <v>151</v>
       </c>
@@ -2630,7 +2633,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
         <v>152</v>
       </c>
@@ -2651,7 +2654,7 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="24" t="s">
         <v>154</v>
       </c>
@@ -2668,7 +2671,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
         <v>155</v>
       </c>
@@ -2685,7 +2688,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
         <v>156</v>
       </c>
@@ -2702,7 +2705,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
         <v>153</v>
       </c>
@@ -2719,7 +2722,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
         <v>20</v>
       </c>
@@ -2739,7 +2742,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
         <v>292</v>
       </c>
@@ -2756,7 +2759,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
         <v>170</v>
       </c>
@@ -2773,7 +2776,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
         <v>38</v>
       </c>
@@ -2793,7 +2796,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
         <v>23</v>
       </c>
@@ -2813,7 +2816,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
         <v>18</v>
       </c>
@@ -2834,7 +2837,7 @@
       </c>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
         <v>265</v>
       </c>
@@ -2854,7 +2857,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="36.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
         <v>142</v>
       </c>
@@ -2874,7 +2877,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>26</v>
       </c>
@@ -2894,7 +2897,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="69" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
         <v>159</v>
       </c>
@@ -2914,7 +2917,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
         <v>176</v>
       </c>
@@ -2931,7 +2934,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="18" t="s">
         <v>169</v>
       </c>
@@ -2948,7 +2951,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
         <v>178</v>
       </c>
@@ -2968,7 +2971,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="69" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
         <v>160</v>
       </c>
@@ -2988,7 +2991,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="18" t="s">
         <v>177</v>
       </c>
@@ -3005,7 +3008,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
         <v>179</v>
       </c>
@@ -3022,7 +3025,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="51.75" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
         <v>28</v>
       </c>
@@ -3042,7 +3045,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="69" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
         <v>161</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
         <v>180</v>
       </c>
@@ -3079,7 +3082,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
         <v>171</v>
       </c>
@@ -3096,7 +3099,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="51.75" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
         <v>29</v>
       </c>
@@ -3116,7 +3119,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="69" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
         <v>162</v>
       </c>
@@ -3136,7 +3139,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
         <v>181</v>
       </c>
@@ -3153,7 +3156,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
         <v>172</v>
       </c>
@@ -3170,7 +3173,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="51.75" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="18" t="s">
         <v>19</v>
       </c>
@@ -3190,7 +3193,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="69" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A55" s="18" t="s">
         <v>157</v>
       </c>
@@ -3210,7 +3213,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
         <v>204</v>
       </c>
@@ -3227,7 +3230,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="18" t="s">
         <v>158</v>
       </c>
@@ -3244,7 +3247,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="18" t="s">
         <v>174</v>
       </c>
@@ -3261,7 +3264,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
         <v>175</v>
       </c>
@@ -3278,7 +3281,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="51.75" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="18" t="s">
         <v>30</v>
       </c>
@@ -3298,7 +3301,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="69" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A61" s="18" t="s">
         <v>163</v>
       </c>
@@ -3318,7 +3321,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="18" t="s">
         <v>182</v>
       </c>
@@ -3335,7 +3338,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="18" t="s">
         <v>173</v>
       </c>
@@ -3352,7 +3355,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="18" t="s">
         <v>185</v>
       </c>
@@ -3372,7 +3375,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="69" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A65" s="18" t="s">
         <v>166</v>
       </c>
@@ -3392,7 +3395,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="18" t="s">
         <v>183</v>
       </c>
@@ -3409,7 +3412,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="18" t="s">
         <v>184</v>
       </c>
@@ -3426,7 +3429,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="18" t="s">
         <v>164</v>
       </c>
@@ -3446,7 +3449,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="18" t="s">
         <v>165</v>
       </c>
@@ -3466,7 +3469,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="18" t="s">
         <v>143</v>
       </c>
@@ -3486,7 +3489,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="86.25" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A71" s="18" t="s">
         <v>186</v>
       </c>
@@ -3504,6 +3507,11 @@
       </c>
       <c r="F71" s="5" t="s">
         <v>294</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="F72" s="5" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -3520,21 +3528,21 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="17.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.3984375" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="105" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.33203125" style="1"/>
+    <col min="4" max="16384" width="9.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
         <v>196</v>
       </c>
@@ -3545,12 +3553,12 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
         <v>71</v>
       </c>
@@ -3558,7 +3566,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
         <v>72</v>
       </c>
@@ -3566,7 +3574,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
         <v>74</v>
       </c>
@@ -3574,7 +3582,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
         <v>73</v>
       </c>
@@ -3582,12 +3590,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>71</v>
       </c>
@@ -3595,7 +3603,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>75</v>
       </c>
@@ -3603,7 +3611,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
         <v>76</v>
       </c>
@@ -3611,7 +3619,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
         <v>74</v>
       </c>
@@ -3619,7 +3627,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>73</v>
       </c>
@@ -3627,12 +3635,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
         <v>77</v>
       </c>
@@ -3640,7 +3648,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>78</v>
       </c>
@@ -3648,7 +3656,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>79</v>
       </c>
@@ -3656,7 +3664,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>80</v>
       </c>
@@ -3664,7 +3672,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>81</v>
       </c>
@@ -3672,7 +3680,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>74</v>
       </c>
@@ -3680,7 +3688,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
         <v>73</v>
       </c>
@@ -3688,12 +3696,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
         <v>82</v>
       </c>
@@ -3701,7 +3709,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
         <v>78</v>
       </c>
@@ -3709,7 +3717,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
         <v>79</v>
       </c>
@@ -3717,7 +3725,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
         <v>80</v>
       </c>
@@ -3725,7 +3733,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
         <v>81</v>
       </c>
@@ -3733,7 +3741,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
         <v>74</v>
       </c>
@@ -3741,7 +3749,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
         <v>73</v>
       </c>
@@ -3749,12 +3757,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
         <v>71</v>
       </c>
@@ -3762,7 +3770,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
         <v>78</v>
       </c>
@@ -3770,7 +3778,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
         <v>79</v>
       </c>
@@ -3778,7 +3786,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
         <v>80</v>
       </c>
@@ -3786,7 +3794,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
         <v>81</v>
       </c>
@@ -3794,7 +3802,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
         <v>74</v>
       </c>
@@ -3802,7 +3810,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
         <v>73</v>
       </c>
@@ -3810,12 +3818,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
         <v>71</v>
       </c>
@@ -3823,7 +3831,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
         <v>78</v>
       </c>
@@ -3831,7 +3839,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>79</v>
       </c>
@@ -3839,7 +3847,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>80</v>
       </c>
@@ -3847,7 +3855,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>81</v>
       </c>
@@ -3855,7 +3863,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>74</v>
       </c>
@@ -3863,7 +3871,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
         <v>73</v>
       </c>
@@ -3871,12 +3879,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
         <v>78</v>
       </c>
@@ -3884,7 +3892,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
         <v>83</v>
       </c>
@@ -3892,7 +3900,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B50" s="1" t="s">
         <v>74</v>
       </c>
@@ -3900,7 +3908,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
         <v>73</v>
       </c>
@@ -3921,14 +3929,14 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="1" max="1" width="35.3984375" customWidth="1"/>
     <col min="2" max="2" width="244" customWidth="1"/>
-    <col min="3" max="3" width="239.1640625" customWidth="1"/>
+    <col min="3" max="3" width="239.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>288</v>
       </c>
@@ -3936,13 +3944,13 @@
         <v>289</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>267</v>
       </c>
       <c r="B4" s="17"/>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>268</v>
       </c>
@@ -3950,7 +3958,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>270</v>
       </c>
@@ -3958,7 +3966,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>272</v>
       </c>
@@ -3966,7 +3974,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>274</v>
       </c>
@@ -3974,7 +3982,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>275</v>
       </c>
@@ -3982,7 +3990,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>277</v>
       </c>
@@ -3990,13 +3998,13 @@
         <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>279</v>
       </c>
       <c r="B11" s="17"/>
     </row>
-    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>280</v>
       </c>
@@ -4004,7 +4012,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>282</v>
       </c>
@@ -4012,7 +4020,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>284</v>
       </c>
@@ -4020,7 +4028,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>286</v>
       </c>

</xml_diff>

<commit_message>
Double checked the data from prediction for establishment costs
</commit_message>
<xml_diff>
--- a/Data/mpatlas_export_nogeo_202503/Field_Definitions 2024_March2024.xlsx
+++ b/Data/mpatlas_export_nogeo_202503/Field_Definitions 2024_March2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessiacosta/Desktop/PhD project/1. Thesis/Ch3. Costs of MPAs/Ch3-MPAcosts/Data/mpatlas_export_nogeo_202503/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessiacosta/Desktop/PhD project/1. Thesis/Ch3. Costs of MPAs/Ch3-p1/Ch3-MPAcosts/Data/mpatlas_export_nogeo_202503/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B66049-3521-2E47-9513-55659C471857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF4349E-76B7-494D-A80D-1F49185ADC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2197,8 +2197,8 @@
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="2" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3412,7 +3412,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="18" t="s">
         <v>184</v>
       </c>

</xml_diff>